<commit_message>
agrego la comparacion de porcentaje vs conc total
</commit_message>
<xml_diff>
--- a/perDW.xlsx
+++ b/perDW.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BA" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="21">
   <si>
     <t>type</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Ergosterol</t>
   </si>
   <si>
+    <t>Sum</t>
+  </si>
+  <si>
     <t>dw</t>
   </si>
   <si>
@@ -90,6 +93,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,10 +175,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -237,10 +241,13 @@
       <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4672.430786</v>
@@ -293,10 +300,13 @@
       <c r="R2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S2" s="0" t="n">
+        <v>6958.92981890816</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>7773.729585</v>
@@ -349,10 +359,13 @@
       <c r="R3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S3" s="0" t="n">
+        <v>12055.0242447</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>453.50449</v>
@@ -405,10 +418,13 @@
       <c r="R4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S4" s="0" t="n">
+        <v>955.51743541604</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>540.837769793765</v>
@@ -461,10 +477,13 @@
       <c r="R5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S5" s="0" t="n">
+        <v>1140.17911605278</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>581.942207596871</v>
@@ -514,10 +533,13 @@
       <c r="R6" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S6" s="0" t="n">
+        <v>1128.65269607797</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2518.32070396535</v>
@@ -570,10 +592,13 @@
       <c r="R7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S7" s="0" t="n">
+        <v>5124.96349911001</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>363.702244432248</v>
@@ -623,10 +648,13 @@
       <c r="R8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S8" s="0" t="n">
+        <v>993.275148730296</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>262.023580350029</v>
@@ -679,10 +707,13 @@
       <c r="R9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S9" s="0" t="n">
+        <v>598.139463201371</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>757.218821029116</v>
@@ -735,10 +766,13 @@
       <c r="R10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S10" s="0" t="n">
+        <v>1541.56185083238</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1556.89220548716</v>
@@ -791,10 +825,13 @@
       <c r="R11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S11" s="0" t="n">
+        <v>3135.79394610158</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>880.100578811176</v>
@@ -847,10 +884,13 @@
       <c r="R12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S12" s="0" t="n">
+        <v>2205.37322034629</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>17974.58421</v>
@@ -903,10 +943,13 @@
       <c r="R13" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S13" s="0" t="n">
+        <v>26260.1658964433</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4044.533779375</v>
@@ -959,10 +1002,13 @@
       <c r="R14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S14" s="0" t="n">
+        <v>12692.698703083</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1584.2623</v>
@@ -1015,10 +1061,13 @@
       <c r="R15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S15" s="0" t="n">
+        <v>3814.705</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3488</v>
@@ -1071,10 +1120,13 @@
       <c r="R16" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S16" s="0" t="n">
+        <v>5400.3857</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3215</v>
@@ -1127,10 +1179,13 @@
       <c r="R17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S17" s="0" t="n">
+        <v>5000.1016</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>16245.12466</v>
@@ -1183,10 +1238,13 @@
       <c r="R18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S18" s="0" t="n">
+        <v>24219.637503994</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1625.71522722212</v>
@@ -1239,10 +1297,13 @@
       <c r="R19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S19" s="0" t="n">
+        <v>3546.27830901935</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>8814.324868</v>
@@ -1295,10 +1356,13 @@
       <c r="R20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S20" s="0" t="n">
+        <v>13343.4920594608</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>721.60910174267</v>
@@ -1351,10 +1415,13 @@
       <c r="R21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S21" s="0" t="n">
+        <v>1548.33980451119</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>501.944855434545</v>
@@ -1407,10 +1474,13 @@
       <c r="R22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S22" s="0" t="n">
+        <v>1095.46633378113</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>676.517085270375</v>
@@ -1460,10 +1530,13 @@
       <c r="R23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S23" s="0" t="n">
+        <v>1586.70461309795</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>5306.30631157449</v>
@@ -1513,10 +1586,13 @@
       <c r="R24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S24" s="0" t="n">
+        <v>11430.2021784593</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>2395.13933587074</v>
@@ -1566,10 +1642,13 @@
       <c r="R25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S25" s="0" t="n">
+        <v>3972.79736073501</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>67.1429502465236</v>
@@ -1622,10 +1701,13 @@
       <c r="R26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S26" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>64.4853915446726</v>
@@ -1678,10 +1760,13 @@
       <c r="R27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S27" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>47.4616656055617</v>
@@ -1734,10 +1819,13 @@
       <c r="R28" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S28" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>47.4344567602771</v>
@@ -1790,10 +1878,13 @@
       <c r="R29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S29" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>51.5607865572022</v>
@@ -1846,10 +1937,13 @@
       <c r="R30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S30" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>49.1383149246366</v>
@@ -1902,10 +1996,13 @@
       <c r="R31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S31" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>36.616464722506</v>
@@ -1958,10 +2055,13 @@
       <c r="R32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S32" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>43.8064358682543</v>
@@ -2014,10 +2114,13 @@
       <c r="R33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S33" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>49.1202361176913</v>
@@ -2070,10 +2173,13 @@
       <c r="R34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S34" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>49.6490596080998</v>
@@ -2126,10 +2232,13 @@
       <c r="R35" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S35" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>39.9071037360734</v>
@@ -2182,10 +2291,13 @@
       <c r="R36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S36" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>68.4480984654956</v>
@@ -2238,10 +2350,13 @@
       <c r="R37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S37" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>31.8650420528189</v>
@@ -2294,10 +2409,13 @@
       <c r="R38" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S38" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>41.5304014334005</v>
@@ -2350,10 +2468,13 @@
       <c r="R39" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S39" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>64.5879793363648</v>
@@ -2406,10 +2527,13 @@
       <c r="R40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S40" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>64.2986934505491</v>
@@ -2462,10 +2586,13 @@
       <c r="R41" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S41" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>67.0741858020008</v>
@@ -2518,10 +2645,13 @@
       <c r="R42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S42" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>45.8428551162325</v>
@@ -2574,10 +2704,13 @@
       <c r="R43" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S43" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>66.0571073053584</v>
@@ -2630,10 +2763,13 @@
       <c r="R44" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S44" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>46.6053446175197</v>
@@ -2686,10 +2822,13 @@
       <c r="R45" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S45" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>45.8201991203167</v>
@@ -2742,10 +2881,13 @@
       <c r="R46" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S46" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>42.6366117351555</v>
@@ -2798,10 +2940,13 @@
       <c r="R47" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S47" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>46.4235560205089</v>
@@ -2854,10 +2999,13 @@
       <c r="R48" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S48" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>60.2884848732283</v>
@@ -2909,6 +3057,9 @@
       </c>
       <c r="R49" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="S49" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2927,10 +3078,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2993,10 +3144,13 @@
       <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00841563</v>
@@ -3049,10 +3203,13 @@
       <c r="R2" s="0" t="n">
         <v>0.015</v>
       </c>
+      <c r="S2" s="0" t="n">
+        <v>3.64249463</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.0126416</v>
@@ -3105,10 +3262,13 @@
       <c r="R3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S3" s="0" t="n">
+        <v>1.0636196</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0122</v>
@@ -3161,10 +3321,13 @@
       <c r="R4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S4" s="0" t="n">
+        <v>4.16276954</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.0122</v>
@@ -3217,10 +3380,13 @@
       <c r="R5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S5" s="0" t="n">
+        <v>4.9376285</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.364</v>
@@ -3273,10 +3439,13 @@
       <c r="R6" s="0" t="n">
         <v>0.22</v>
       </c>
+      <c r="S6" s="0" t="n">
+        <v>69.962389</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.13845</v>
@@ -3329,10 +3498,13 @@
       <c r="R7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S7" s="0" t="n">
+        <v>31.7283018</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.7545</v>
@@ -3385,10 +3557,13 @@
       <c r="R8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S8" s="0" t="n">
+        <v>89.3505</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.512</v>
@@ -3441,10 +3616,13 @@
       <c r="R9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S9" s="0" t="n">
+        <v>74.15866</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1.66351515740336</v>
@@ -3497,10 +3675,13 @@
       <c r="R10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S10" s="0" t="n">
+        <v>68.185558876656</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.48</v>
@@ -3553,10 +3734,13 @@
       <c r="R11" s="0" t="n">
         <v>3.21667601440568</v>
       </c>
+      <c r="S11" s="0" t="n">
+        <v>17.7678461917401</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1.5</v>
@@ -3609,10 +3793,13 @@
       <c r="R12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S12" s="0" t="n">
+        <v>120.560257036891</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0174651905815287</v>
@@ -3665,10 +3852,13 @@
       <c r="R13" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S13" s="0" t="n">
+        <v>3.28581303066362</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.87</v>
@@ -3721,10 +3911,13 @@
       <c r="R14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S14" s="0" t="n">
+        <v>210.109047509172</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.35</v>
@@ -3777,10 +3970,13 @@
       <c r="R15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S15" s="0" t="n">
+        <v>28.691289767863</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.2057</v>
@@ -3833,10 +4029,13 @@
       <c r="R16" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S16" s="0" t="n">
+        <v>37.3747772320192</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.7451</v>
@@ -3889,10 +4088,13 @@
       <c r="R17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S17" s="0" t="n">
+        <v>43.4419257675166</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.256290070804651</v>
@@ -3945,10 +4147,13 @@
       <c r="R18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S18" s="0" t="n">
+        <v>11.1578529651646</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.157966917009894</v>
@@ -4001,10 +4206,13 @@
       <c r="R19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S19" s="0" t="n">
+        <v>44.190298238337</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.342678276399</v>
@@ -4057,10 +4265,13 @@
       <c r="R20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S20" s="0" t="n">
+        <v>25.8916144346342</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.268100569298955</v>
@@ -4113,10 +4324,13 @@
       <c r="R21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S21" s="0" t="n">
+        <v>4.54357722839748</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.274838168122783</v>
@@ -4169,10 +4383,13 @@
       <c r="R22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S22" s="0" t="n">
+        <v>15.8778727583269</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.0331384376767369</v>
@@ -4225,10 +4442,13 @@
       <c r="R23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S23" s="0" t="n">
+        <v>13.4920746063118</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.126445268943807</v>
@@ -4281,10 +4501,13 @@
       <c r="R24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S24" s="0" t="n">
+        <v>4.99361502436643</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.535322032720861</v>
@@ -4337,10 +4560,13 @@
       <c r="R25" s="0" t="n">
         <v>4.5426442084437</v>
       </c>
+      <c r="S25" s="0" t="n">
+        <v>56.8842268832064</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.415990409340632</v>
@@ -4393,10 +4619,13 @@
       <c r="R26" s="0" t="n">
         <v>0.295910085711765</v>
       </c>
+      <c r="S26" s="0" t="n">
+        <v>31.0155893805796</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.32860834302005</v>
@@ -4449,10 +4678,13 @@
       <c r="R27" s="0" t="n">
         <v>0.0940728519401797</v>
       </c>
+      <c r="S27" s="0" t="n">
+        <v>111.940991000705</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.23110426412406</v>
@@ -4505,10 +4737,13 @@
       <c r="R28" s="0" t="n">
         <v>0.00715772107197407</v>
       </c>
+      <c r="S28" s="0" t="n">
+        <v>50.6697529734385</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.205105039964668</v>
@@ -4561,10 +4796,13 @@
       <c r="R29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S29" s="0" t="n">
+        <v>10.0044227591002</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.164995568869331</v>
@@ -4617,10 +4855,13 @@
       <c r="R30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S30" s="0" t="n">
+        <v>13.5172415751479</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.1288315905977</v>
@@ -4673,10 +4914,13 @@
       <c r="R31" s="0" t="n">
         <v>1.26585120210948</v>
       </c>
+      <c r="S31" s="0" t="n">
+        <v>74.756354115002</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.382025596918642</v>
@@ -4729,10 +4973,13 @@
       <c r="R32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S32" s="0" t="n">
+        <v>8.79824446489931</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.0983728898345733</v>
@@ -4785,10 +5032,13 @@
       <c r="R33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S33" s="0" t="n">
+        <v>4.14390519354181</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0.135915575793596</v>
@@ -4841,10 +5091,13 @@
       <c r="R34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S34" s="0" t="n">
+        <v>14.1170007787346</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0.231040285706612</v>
@@ -4897,10 +5150,13 @@
       <c r="R35" s="0" t="n">
         <v>0.411805686038856</v>
       </c>
+      <c r="S35" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1.18854522801197</v>
@@ -4953,10 +5209,13 @@
       <c r="R36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S36" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.293074115267981</v>
@@ -5009,10 +5268,13 @@
       <c r="R37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S37" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.247082177203084</v>
@@ -5065,10 +5327,13 @@
       <c r="R38" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S38" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0.520279546200173</v>
@@ -5121,10 +5386,13 @@
       <c r="R39" s="0" t="n">
         <v>0.314454670780324</v>
       </c>
+      <c r="S39" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0.436361204809266</v>
@@ -5177,10 +5445,13 @@
       <c r="R40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S40" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0.844427283563047</v>
@@ -5233,10 +5504,13 @@
       <c r="R41" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S41" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.690411612076054</v>
@@ -5289,10 +5563,13 @@
       <c r="R42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S42" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>2.43968838095552</v>
@@ -5345,10 +5622,13 @@
       <c r="R43" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S43" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>2.70150920274818</v>
@@ -5401,10 +5681,13 @@
       <c r="R44" s="0" t="n">
         <v>18.1039163649506</v>
       </c>
+      <c r="S44" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1.24419110979583</v>
@@ -5457,10 +5740,13 @@
       <c r="R45" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S45" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.591727038093178</v>
@@ -5513,10 +5799,13 @@
       <c r="R46" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S46" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.414070698198764</v>
@@ -5569,10 +5858,13 @@
       <c r="R47" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S47" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1.21988242017629</v>
@@ -5625,10 +5917,13 @@
       <c r="R48" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S48" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0.550371173379933</v>
@@ -5681,10 +5976,13 @@
       <c r="R49" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S49" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1.71516337463369</v>
@@ -5737,10 +6035,13 @@
       <c r="R50" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S50" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>2.29694791287179</v>
@@ -5793,10 +6094,13 @@
       <c r="R51" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S51" s="0" t="n">
+        <v>99.9999999999999</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0.357469678430119</v>
@@ -5849,10 +6153,13 @@
       <c r="R52" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S52" s="0" t="n">
+        <v>99.9999999999999</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1.32351065733704</v>
@@ -5905,10 +6212,13 @@
       <c r="R53" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S53" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>5.90064955038772</v>
@@ -5961,10 +6271,13 @@
       <c r="R54" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S54" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1.73095081630912</v>
@@ -6017,10 +6330,13 @@
       <c r="R55" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S55" s="0" t="n">
+        <v>99.9999999999999</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0.245614100452975</v>
@@ -6073,10 +6389,13 @@
       <c r="R56" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S56" s="0" t="n">
+        <v>99.9999999999999</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>2.53213890792172</v>
@@ -6129,10 +6448,13 @@
       <c r="R57" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S57" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0.941072880923519</v>
@@ -6185,10 +6507,13 @@
       <c r="R58" s="0" t="n">
         <v>7.98577120116367</v>
       </c>
+      <c r="S58" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1.34123006413383</v>
@@ -6241,10 +6566,13 @@
       <c r="R59" s="0" t="n">
         <v>0.954068878333322</v>
       </c>
+      <c r="S59" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0.293554970420067</v>
@@ -6297,10 +6625,13 @@
       <c r="R60" s="0" t="n">
         <v>0.084037894518539</v>
       </c>
+      <c r="S60" s="0" t="n">
+        <v>99.9999999999999</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0.456099054292226</v>
@@ -6353,10 +6684,13 @@
       <c r="R61" s="0" t="n">
         <v>0.0141262205792205</v>
       </c>
+      <c r="S61" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>2.05014367048913</v>
@@ -6409,10 +6743,13 @@
       <c r="R62" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S62" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>1.22063046629783</v>
@@ -6465,10 +6802,13 @@
       <c r="R63" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S63" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0.172335304634454</v>
@@ -6521,10 +6861,13 @@
       <c r="R64" s="0" t="n">
         <v>1.69330248524714</v>
       </c>
+      <c r="S64" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4.34206617516412</v>
@@ -6577,10 +6920,13 @@
       <c r="R65" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S65" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>2.37391748218288</v>
@@ -6633,10 +6979,13 @@
       <c r="R66" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="S66" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0.962779402820005</v>
@@ -6688,12 +7037,15 @@
       </c>
       <c r="R67" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="S67" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>